<commit_message>
added some new stuff to sysrequirements
</commit_message>
<xml_diff>
--- a/Design/system requirements.xlsx
+++ b/Design/system requirements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anmol\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anmol\Desktop\OrderBook Group Git\order-book-project-team-3\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7524B6A-16AD-4D38-AEC2-FEBF2F5FF761}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A41AE2-C410-43F7-8DCA-1215AC987FD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="92">
   <si>
     <t>High-level Requirements</t>
   </si>
@@ -297,9 +297,6 @@
     <t>Under Review</t>
   </si>
   <si>
-    <t>RJ</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -337,6 +334,42 @@
   </si>
   <si>
     <t>In-Progress</t>
+  </si>
+  <si>
+    <t>HLR_009</t>
+  </si>
+  <si>
+    <t>Order Processing</t>
+  </si>
+  <si>
+    <t>Show Status</t>
+  </si>
+  <si>
+    <t>System must add Order Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System must add an Order Status "Buy" or "Sell  to the order created. </t>
+  </si>
+  <si>
+    <t>Processing</t>
+  </si>
+  <si>
+    <t>HLR_010</t>
+  </si>
+  <si>
+    <t>Party ID</t>
+  </si>
+  <si>
+    <t>An admin must be able to add the Party ID</t>
+  </si>
+  <si>
+    <t>The admin must be able to assign a Party ID to the order</t>
+  </si>
+  <si>
+    <t>HLR_001,002</t>
+  </si>
+  <si>
+    <t>HLR_011</t>
   </si>
 </sst>
 </file>
@@ -893,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1403,13 +1436,13 @@
         <v>66</v>
       </c>
       <c r="M13" s="23" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="N13" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O13" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P13" s="21" t="s">
         <v>34</v>
@@ -1417,25 +1450,25 @@
     </row>
     <row r="14" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="E14" s="18" t="s">
         <v>71</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>72</v>
       </c>
       <c r="F14" s="20">
         <v>1</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H14" s="23" t="s">
         <v>27</v>
@@ -1444,65 +1477,131 @@
         <v>28</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K14" s="23" t="s">
         <v>34</v>
       </c>
       <c r="L14" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M14" s="23" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="N14" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O14" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P14" s="21" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="21"/>
+      <c r="A15" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="20">
+        <v>1</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="M15" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="N15" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O15" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="P15" s="21" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="21"/>
+      <c r="A16" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="20">
+        <v>1</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="L16" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="M16" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="N16" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O16" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="P16" s="21" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="17" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="16"/>
+      <c r="A17" s="16" t="s">
+        <v>91</v>
+      </c>
       <c r="B17" s="16"/>
       <c r="C17" s="20"/>
       <c r="D17" s="25"/>
@@ -1864,7 +1963,7 @@
     <row r="37" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A37" s="33"/>
       <c r="B37" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C37" s="35"/>
       <c r="D37" s="36"/>
@@ -1887,10 +1986,10 @@
         <v>16</v>
       </c>
       <c r="C38" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="40" t="s">
         <v>76</v>
-      </c>
-      <c r="D38" s="40" t="s">
-        <v>77</v>
       </c>
       <c r="E38" s="31"/>
       <c r="F38" s="31"/>
@@ -1932,7 +2031,7 @@
     <row r="40" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A40" s="41"/>
       <c r="B40" s="41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C40" s="42" t="s">
         <v>65</v>
@@ -1956,10 +2055,10 @@
     <row r="41" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A41" s="41"/>
       <c r="B41" s="41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C41" s="42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D41" s="43">
         <v>3</v>
@@ -1980,7 +2079,7 @@
     <row r="42" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A42" s="41"/>
       <c r="B42" s="41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C42" s="31"/>
       <c r="D42" s="43">
@@ -2956,7 +3055,7 @@
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L13:L18 L21:L34" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L21:L34 L13:L14 L16:L18 L15" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Status</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L7:L12 L19:L20" xr:uid="{00000000-0002-0000-0000-000001000000}">

</xml_diff>